<commit_message>
added personalized distribution of salary
</commit_message>
<xml_diff>
--- a/MoneyControl.xlsx
+++ b/MoneyControl.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tushar\Documents\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tushar\Documents\Projects\MoneyControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,13 +19,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">
+                                                                      Enter values to cell colored in --&gt;</t>
+  </si>
+  <si>
+    <t>Split of Salary in (%)</t>
+  </si>
+  <si>
+    <t>Split of Investment Amount in (%)</t>
+  </si>
+  <si>
+    <t>Split of Equity Amount in (%)</t>
+  </si>
+  <si>
+    <t>Increase in each after Salary change in (%)</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Wants</t>
+  </si>
+  <si>
+    <t>Invest</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Debt</t>
+  </si>
+  <si>
+    <t>Index Fund</t>
+  </si>
+  <si>
+    <t>Flexi Fund</t>
+  </si>
+  <si>
+    <t>Mid Cap</t>
+  </si>
+  <si>
+    <t>Small Cap</t>
+  </si>
   <si>
     <t xml:space="preserve">Salary </t>
   </si>
   <si>
     <t>Date
-(YYYY-MM-DD)</t>
+(DD-MM-YY)</t>
   </si>
   <si>
     <t>Salary Increment</t>
@@ -34,38 +77,14 @@
     <t>% Increase</t>
   </si>
   <si>
-    <t>Monthly Expenses</t>
-  </si>
-  <si>
-    <t>Wants</t>
-  </si>
-  <si>
-    <t>Invest</t>
-  </si>
-  <si>
-    <t>Equity</t>
-  </si>
-  <si>
-    <t>Debt</t>
-  </si>
-  <si>
-    <t>Index Fund</t>
-  </si>
-  <si>
     <t>Flexi Cap</t>
-  </si>
-  <si>
-    <t>Mid Cap</t>
-  </si>
-  <si>
-    <t>Small Cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,10 +92,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -97,8 +117,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,22 +166,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -148,6 +215,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -161,44 +243,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
+    <cellStyle name="Accent5" xfId="5" builtinId="45"/>
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -413,128 +578,451 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.21875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" style="4" customWidth="1"/>
-    <col min="11" max="11" width="0.21875" style="8" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.21875" style="4" customWidth="1"/>
-    <col min="16" max="29" width="8.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5546875" style="13" customWidth="1"/>
+    <col min="10" max="11" width="7.44140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" style="13" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="31" width="8.6640625" style="13" customWidth="1"/>
+    <col min="32" max="38" width="14.44140625" style="13" customWidth="1"/>
+    <col min="39" max="16384" width="14.44140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:25" s="12" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="T1" s="19"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O2" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="P2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1">
-        <f>A2</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="4">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4">
+        <v>30</v>
+      </c>
+      <c r="H3" s="4">
+        <v>20</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="4">
+        <v>60</v>
+      </c>
+      <c r="K3" s="4">
+        <v>40</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="4">
+        <v>40</v>
+      </c>
+      <c r="N3" s="4">
+        <v>25</v>
+      </c>
+      <c r="O3" s="4">
+        <v>20</v>
+      </c>
+      <c r="P3" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="4">
+        <v>20</v>
+      </c>
+      <c r="T3" s="4">
+        <v>30</v>
+      </c>
+      <c r="U3" s="4">
+        <v>50</v>
+      </c>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="18" t="str">
+        <f>IF(SUM(F3:H3) = 100, "Split is Correct", "Split is Incorrect")</f>
+        <v>Split is Correct</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="18" t="str">
+        <f>IF(SUM(J3:K3) = 100, "Split is Correct", "Split is Incorrect")</f>
+        <v>Split is Correct</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="18" t="str">
+        <f>IF(SUM(M3:P3) = 100, "Split is Correct", "Split is Incorrect")</f>
+        <v>Split is Correct</v>
+      </c>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="18" t="str">
+        <f>IF(SUM(S3:U3) = 100, "Split is Correct", "Split is Incorrect")</f>
+        <v>Split is Correct</v>
+      </c>
+      <c r="T4" s="19"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+    </row>
+    <row r="7" spans="1:25" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>28844</v>
+      </c>
+      <c r="B8" s="8">
+        <v>44734</v>
+      </c>
+      <c r="C8" s="7">
+        <f>A8</f>
+        <v>28844</v>
+      </c>
+      <c r="D8" s="7">
         <v>100</v>
       </c>
-      <c r="E2" s="1">
-        <f>(A2*0.5)</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <f>(ROUNDDOWN((A2*0.3),0))</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <f>ROUNDUP((A2*0.2),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="3">
-        <f>ROUNDUP(G2*0.6,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <f>ROUNDDOWN(G2* 0.4,0)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="3">
-        <f>ROUNDUP(I2*0.4,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <f>ROUNDUP(I2*0.25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <f>ROUNDDOWN(I2* 0.2, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="3">
-        <f>ROUNDDOWN(I2* 0.15, 0)</f>
-        <v>0</v>
+      <c r="F8" s="7">
+        <f>(A8*(F3/100))</f>
+        <v>14422</v>
+      </c>
+      <c r="G8" s="10">
+        <f>(ROUNDDOWN((A8*G3/100),0))</f>
+        <v>8653</v>
+      </c>
+      <c r="H8" s="10">
+        <f>ROUNDUP((A8*H3/100),0)</f>
+        <v>5769</v>
+      </c>
+      <c r="J8" s="10">
+        <f>ROUNDUP(H8*J3/100,0)</f>
+        <v>3462</v>
+      </c>
+      <c r="K8" s="10">
+        <f>ROUNDDOWN(H8* K3/100,0)</f>
+        <v>2307</v>
+      </c>
+      <c r="M8" s="10">
+        <f>ROUNDUP(J8*M3/100,0)</f>
+        <v>1385</v>
+      </c>
+      <c r="N8" s="10">
+        <f>ROUNDUP(J8*N3/100,0)</f>
+        <v>866</v>
+      </c>
+      <c r="O8" s="10">
+        <f>ROUNDDOWN(J8* O3/100, 0)</f>
+        <v>692</v>
+      </c>
+      <c r="P8" s="10">
+        <f>ROUNDDOWN(J8* P3/100, 0)</f>
+        <v>519</v>
+      </c>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="V8" s="11"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>47811</v>
+      </c>
+      <c r="B9" s="22">
+        <v>44877</v>
+      </c>
+      <c r="C9">
+        <f>(A9-A8)</f>
+        <v>18967</v>
+      </c>
+      <c r="D9">
+        <f>ROUND((C9/A8)*100,0)</f>
+        <v>66</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9">
+        <f>ROUNDDOWN((F8+(C9*S3/100)),0)</f>
+        <v>18215</v>
+      </c>
+      <c r="G9">
+        <f>ROUNDDOWN((G8+(C9*T3/100)),0)</f>
+        <v>14343</v>
+      </c>
+      <c r="H9">
+        <f>ROUNDUP((H8+(C9*U3/100)),0)</f>
+        <v>15253</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9">
+        <f>ROUNDUP(H9*J3/100,0)</f>
+        <v>9152</v>
+      </c>
+      <c r="K9">
+        <f>ROUNDDOWN(H9*K3/100,0)</f>
+        <v>6101</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9">
+        <f>ROUNDUP(J9*M3/100,0)</f>
+        <v>3661</v>
+      </c>
+      <c r="N9">
+        <f>ROUNDUP(J9*N3/100,0)</f>
+        <v>2288</v>
+      </c>
+      <c r="O9">
+        <f>ROUNDDOWN(J9*O3/100,0)</f>
+        <v>1830</v>
+      </c>
+      <c r="P9">
+        <f>ROUNDDOWN(J9*P3/100,0)</f>
+        <v>1372</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576 K1:K1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="black">
-      <formula>NOT(ISERROR(SEARCH("black",H1)))</formula>
+  <mergeCells count="17">
+    <mergeCell ref="V1:Y6"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="M5:P6"/>
+    <mergeCell ref="S5:U6"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A1:E6"/>
+    <mergeCell ref="F5:H6"/>
+    <mergeCell ref="I1:I6"/>
+    <mergeCell ref="L1:L6"/>
+    <mergeCell ref="Q1:R6"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F4:H4 J4:K4 M4:P4 S4:U4">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Incorrect">
+      <formula>NOT(ISERROR(SEARCH("Incorrect",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Correct">
+      <formula>NOT(ISERROR(SEARCH("Correct",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>